<commit_message>
Fix format and solve logging bug
</commit_message>
<xml_diff>
--- a/output/search_result.xlsx
+++ b/output/search_result.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,15 +459,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Africa's cholera crisis worsens amid extreme weather events ...</t>
+          <t>See full schedule</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45436</v>
+        <v>45447</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Billions of dollars have been invested into other diseases that predominantly affect the world's most vulnerable, like polio and</t>
+          <t>Beyond the headlines to the heart of the news of the day. Al Jazeera gets the Inside Story from some of the best minds in the Middle East and beyond.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -485,15 +485,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Russia-Ukraine war updates: Ukraine's east sees most intensive ...</t>
+          <t>Migration | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>A landmark European Union decision this week to send Ukraine the interest earned by hundreds of billions of dollars in Russian central bank</t>
+          <t>Order will allow US to shut off asylum requests and deny entry to migrants once daily threshold met, US media reporting. Published On 3 Jun 20243 Jun</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -511,15 +511,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nvidia's profits soar as AI boom shows no sign of slowing down ...</t>
+          <t>Latin America News | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>45434</v>
+        <v>45445</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>“Companies and countries are partnering with Nvidia to shift the trillion-dollar   Forecast beat expectations by billions of dollars, a</t>
+          <t>Sheinbaum's resounding win offers a bright spot for the Latin American left amid a string of setbacks.   Claudia Sheinbaum pumps her fist as she acknowledges</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -528,7 +528,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -537,15 +537,15 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>'New ground is being broken': EU seizes Russian profits for Ukraine ...</t>
+          <t>Leaders praise 'historic' victory as Sheinbaum triumphs in Mexican ...</t>
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>45435</v>
+        <v>45447</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>A landmark EU decision this week to send Ukraine the interest earned by hundreds of billions of dollars in Russian central bank accounts on</t>
+          <t>By contrast, in countries like Colombia and Chile, left-leaning presidents have seen their popularity ebb as they struggle to make progress on</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -563,15 +563,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Singapore Airlines death: Is climate change making air turbulence ...</t>
+          <t>Mexico's election puts Lopez Obrador's stance on Israel under ...</t>
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>45435</v>
+        <v>45445</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>But these lawsuits put a strain on airlines because the industry has fairly tight margins, meaning every dollar matters. In December the</t>
+          <t>In Colombia, meanwhile, Gustavo Petro became the first left-wing leader to win the modern presidency.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -589,15 +589,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Israel's war on Gaza live news: Attacks on besieged enclave kill 62 ...</t>
+          <t>Brazil withdraws ambassador to Israel after Gaza war criticism ...</t>
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>45434</v>
+        <v>45441</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Israel, a major recipient of US military assistance for decades, is still due to receive billions of dollars of US aid and weaponry. “The</t>
+          <t>Colombian President Gustavo Petro, who has also severed ties with Israel. Both Brazil and Colombia have supported South Africa's complaint</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -615,15 +615,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Israel's war on Gaza live news: Deadly combat rages as Rafah ...</t>
+          <t>Colombia lawmakers pass bullfighting ban | News | Al Jazeera</t>
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>45434</v>
+        <v>45441</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Israel, a major recipient of US military assistance for decades, is still due to receive billions of dollars of US aid and weaponry. “The</t>
+          <t>Colombia's Congress has passed legislation banning bullfighting. Lawmakers passed the bill 93-2 on Tuesday. Activists have spent many years</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -641,15 +641,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gaza war: What does victory look like for the US and Israel? | Israel ...</t>
+          <t>Colombia's ex-President Uribe charged with witness tampering ...</t>
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>45433</v>
+        <v>45436</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Israel has said it is seeking an “absolute victory” over Hamas, as it continues to receive billions of dollars in unconditional military aid</t>
+          <t>Former Colombia President Alvaro Uribe. Uribe, who was president from 2002 to 2010, has denied any wrongdoing and has accused Colombia's</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -667,15 +667,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Israel's war on Gaza live: UNRWA suspends food distribution in Rafah</t>
+          <t>'Major non-NATO ally': What does Biden's new Kenya pledge mean ...</t>
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>45432</v>
+        <v>45435</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dollars in US military assistance that remains in the pipeline for Prime Minister Benjamin Netanyahu's government. But Biden has also faced</t>
+          <t>The US has currently designated 18 countries as MNNAs. These include Argentina, Australia, Bahrain, Brazil, Colombia, Egypt, Israel, Japan,</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -693,15 +693,15 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>'We love Taiwan': Domestic workers hope for more from new ...</t>
+          <t>Why is Israel angry some EU countries are recognising Palestine ...</t>
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>45432</v>
+        <v>45434</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>While Taiwan's monthly minimum salary was increased to 27,470 New Taiwan dollars ($853) this year, migrant domestic workers, who also have to</t>
+          <t>Colombia's Petro orders opening of embassy in West Bank's Ramallah. Petro had recalled the Colombian ambassador from Tel Aviv, where the</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -710,24 +710,24 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Who died alongside Iran's President Raisi in the helicopter crash ...</t>
+          <t>Colombia's Petro orders opening of embassy in West Bank's ...</t>
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>45432</v>
+        <v>45434</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>The AQR is a colossal bonyad, or charitable trust, that has billions of dollars in assets and is the custodian of the shrine of Imam Reza</t>
+          <t>Colombian President Gustavo Petro has ordered the opening of an embassy in the Palestinian city of Ramallah, Foreign Minister Luis Gilberto</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -745,15 +745,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Iran helicopter crash updates: President Raisi, FM Amirabdollahian ...</t>
+          <t>The ICC is not in the business of peacemaking, but it can deliver ...</t>
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>45431</v>
+        <v>45434</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>dollars, according to a Reuters investigation. Under Mokhber's watch, Setad developed Iran's coronavirus vaccine, Coviran Barekat, at the</t>
+          <t>But more “complicated” peace negotiations do not necessarily mean “worse” peace negotiations. Take Colombia, for example, where the ICC had a</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -771,15 +771,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Who is Mohammad Mokhber, Iran's interim president? | Politics ...</t>
+          <t>Mapping which countries recognise Palestine in 2024 | Israel ...</t>
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>45432</v>
+        <v>45433</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Mokhber led the Iranian supreme leader's multibillion-dollar charitable conglomerate for 14 years.</t>
+          <t>Colombia. 2015: Saint Lucia. 2014: Sweden. 2013: Guatemala, Haiti, the Vatican. 2012: Thailand. 2011: Chile, Guyana, Peru, Suriname, Uruguay</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -788,7 +788,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -797,15 +797,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ebrahim Raisi, Iran's president, dies in helicopter crash aged 63 ...</t>
+          <t>Are seed-sowing drones the answer to global deforestation ...</t>
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>45431</v>
+        <v>45429</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>The colossal bonyad, or charitable trust, has billions of dollars in assets and is the custodian of the shrine of Imam Reza, the eighth Shia</t>
+          <t>And, in Colombia, internal violence and displacement have pushed armed groups, farmers and cattle farmers into the forests, causing more</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -823,15 +823,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Panic in Bishkek: Why were Pakistani students attacked in ...</t>
+          <t>Colombia hunts for assailants after Bogota prison director shot dead ...</t>
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>45432</v>
+        <v>45428</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>The Pakistani rupee, which stood at 160 against the US dollar in December 2020, has since slipped by more than 70 percent to 278 rupees a dollar</t>
+          <t>The new director of one of Colombia's biggest prisons has been shot dead, the authorities said, after receiving threats against him and his</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -849,15 +849,15 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Week in pictures: From a Putin-Xi meeting to Cannes Film Festival ...</t>
+          <t>Children of the Darien Gap | Migration | Al Jazeera</t>
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>45431</v>
+        <v>45419</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>dollars in US military aid are on their way to the country and would make a 'real difference' on the battlefield. [Brendan Smialowski/Pool</t>
+          <t>Colombia and Panama that is the only land route for migrants heading north from South America. Amid historic regional migration and new</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -875,15 +875,15 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Russian court seizes two European banks' assets amid Western ...</t>
+          <t>Colombia president cuts ties with Israel over war on Gaza | Israel ...</t>
         </is>
       </c>
       <c r="B18" s="1" t="n">
-        <v>45430</v>
+        <v>45413</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Freezing hundreds of billions of dollars in lenders' assets was part of dispute over gas project halted by sanctions.</t>
+          <t>Colombia's President Gustavo Petro says the country is cutting diplomatic ties with Israel over its war on Gaza.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -901,15 +901,15 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Lebanon's economic crisis endures, as does the EU's 'fear' of ...</t>
+          <t>Arrests at Columbia University as New York City police clear Gaza ...</t>
         </is>
       </c>
       <c r="B19" s="1" t="n">
-        <v>45430</v>
+        <v>45412</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Billions of dollars go to the Syrian government, leaving it at the centre of the amphetamine's trade. Published On 10 Mar 202410 Mar 2024.</t>
+          <t>Violent clashes erupt at UCLA between pro-Palestinian protesters and pro-Israeli counter-demonstrators.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -918,7 +918,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -927,15 +927,15 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>What is Trident, the US floating pier off Gaza? Will it work? | Israel ...</t>
+          <t>Colombia to cut diplomatic ties with Israel over Gaza war, Petro says ...</t>
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>45428</v>
+        <v>45412</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Washington has provided billions of dollars in aid as well as weapons that Israel has used in Gaza since October 7. Source: Al Jazeera</t>
+          <t>Colombia to cut diplomatic ties with Israel over Gaza war, Petro says. Colombian President Gustavo Petro, a staunch critic of Israel's war in</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -944,7 +944,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -953,15 +953,15 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Western volunteers join the battle against Myanmar's military regime ...</t>
+          <t>Huge crowds protest Colombian president's planned reforms ...</t>
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>45428</v>
+        <v>45403</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>dollar arsenal supplied by Russia and China. Ethnic armies, public donations and weapon seizures partly as a result of last year's Operation</t>
+          <t>Huge crowds protest Colombian president's planned reforms. Protesters call Gustavo Petro's policies 'dire' as his government attempts to reform</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -979,15 +979,15 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Republicans in US House pass bill pushing Biden to send weapons ...</t>
+          <t>Former Colombian President Alvaro Uribe blasts impending criminal ...</t>
         </is>
       </c>
       <c r="B22" s="1" t="n">
-        <v>45428</v>
+        <v>45391</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Israel, a major recipient of US military assistance for decades, is still due to get billions of dollars of US weaponry, despite the delay</t>
+          <t>Prosecutors announced this week they intended to pursue the right-wing Uribe on charges of witness tampering and fraud.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1005,15 +1005,15 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Anxious Zimbabwean migrants, smugglers watch South Africa's ...</t>
+          <t>Forced from home, these Colombians struggle to live in a basketball ...</t>
         </is>
       </c>
       <c r="B23" s="1" t="n">
-        <v>45426</v>
+        <v>45391</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>The border province even favours using the South African rand, which people prefer to the local currency or the US dollar, which is popular</t>
+          <t>Forced from home, Colombians build a life in a basketball stadium · An invisible crisis · A sanctuary from gunfire · Resources stretched thin.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1031,15 +1031,15 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Biden administration plans to send $1bn in military aid to Israel ...</t>
+          <t>Colombia seeks to join Gaza genocide case against Israel at ICJ ...</t>
         </is>
       </c>
       <c r="B24" s="1" t="n">
-        <v>45426</v>
+        <v>45386</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Request for tank ammunition, tactical vehicles for Israel despite Biden's earlier pause on bombs over Rafah assault.</t>
+          <t>Colombia seeks to join Gaza genocide case against Israel at ICJ. Bogota calls on the World Court to ensure 'the safety' and 'the very existence</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1048,24 +1048,24 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Russia's defence rejig: 'Unfortunately for Ukraine, a very effective ...</t>
+          <t>Colombia and Panama failing to protect migrants in Darien Gap ...</t>
         </is>
       </c>
       <c r="B25" s="1" t="n">
-        <v>45425</v>
+        <v>45384</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>dollars on new weaponry and payments to servicemen and their families. “Putin needs an 'arsenal of autocracy' that can outperform Ukraine</t>
+          <t>In a report on Wednesday, the rights group said the Colombian and Panamanian authorities have not protected people transiting through the Darien</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1074,7 +1074,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -1083,15 +1083,15 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Not even the US government knows the US government line on ...</t>
+          <t>Colombia expels Argentina's diplomats after Milei calls Petro ...</t>
         </is>
       </c>
       <c r="B26" s="1" t="n">
-        <v>45425</v>
+        <v>45378</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Of course, this money was authorised on top of the billions of dollars that the US already sends the country on an annual basis. When on May</t>
+          <t>Colombia expels Argentina's diplomats after Milei calls Petro 'terrorist'. Argentina's president calls his Colombian counterpart a 'terrorist',</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1100,7 +1100,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -1109,15 +1109,15 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Boeing's jets turn 70: A timeline of highs, lows and turbulence ...</t>
+          <t>Tonnes of cocaine seized after high-speed boat chase in Colombia ...</t>
         </is>
       </c>
       <c r="B27" s="1" t="n">
-        <v>45425</v>
+        <v>45377</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>That same model rocket would be used for the Apollo 11 mission in 1969, landing astronauts on the moon. Boeing, the billion-dollar company.</t>
+          <t>Over five tonnes of cocaine have been seized in Colombia after two drug bust operations that involved a boat chase.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1126,7 +1126,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -1135,15 +1135,15 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>One of the biggest hurdles for athletes on the Olympic path: Money ...</t>
+          <t>In Colombia, hunting poachers, not drug traffickers | Wildlife News ...</t>
         </is>
       </c>
       <c r="B28" s="1" t="n">
-        <v>45424</v>
+        <v>45371</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>She declined to share the dollar figure for those costs as well. Lozano told Al Jazeera that she's using the funds from her GoFundMe campaign to</t>
+          <t>One of the most biodiverse countries in the world, Colombia is increasingly vulnerable to illicit wildlife trafficking; in 2023, the wildlife</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -1161,15 +1161,15 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>US university ties to weapons contractors under scrutiny amid war in ...</t>
+          <t>Colombia names attorney general amid political unrest under ...</t>
         </is>
       </c>
       <c r="B29" s="1" t="n">
-        <v>45424</v>
+        <v>45362</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Many student demonstrators have zeroed in on their schools' multimillion-dollar endowment funds as a target for their activism. Those financial</t>
+          <t>Colombia names attorney general amid political unrest under Gustavo Petro. Luz Adriana Camargo Garzon will lead probes into President Petro and</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1178,166 +1178,10 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>What did Biden say about US arms transfers to Israel and what does ...</t>
-        </is>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>45420</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>The US sends Israel $3.8bn in military aid annually, and Congress recently approved billions of dollars in additional support for the country.</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>./output/28.jpg</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>After decades of decline, Air India is betting billions on a comeback ...</t>
-        </is>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>45420</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>In recent decades, India's national airline came to be seen as a cautionary tale of decline as it racked up billions of dollars in losses and</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>./output/29.jpg</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Pentagon chief confirms US pause on weapons shipment to Israel ...</t>
-        </is>
-      </c>
-      <c r="B32" s="1" t="n">
-        <v>45419</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Over the years, the United States has provided tens of billions of dollars in military aid to Israel.” 'Iron-clad' support. The Biden</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>./output/30.jpg</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
-        <v>1</v>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Zimbabwe's illegal forex dealers use WhatsApp to find clients, evade ...</t>
-        </is>
-      </c>
-      <c r="B33" s="1" t="n">
-        <v>45418</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Everyone from state utilities to street vendors accepts payment in US dollars. Because of the popularity of the greenback, black market forex</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>./output/31.jpg</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
-        <v>1</v>
-      </c>
-      <c r="F33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Boeing postpones launch of Starliner space capsule after technical ...</t>
-        </is>
-      </c>
-      <c r="B34" s="1" t="n">
-        <v>45418</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>NASA in 2014 awarded multibillion-dollar contracts to Boeing and SpaceX to develop space capsules for the space agency to ferry astronauts and</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>./output/32.jpg</t>
-        </is>
-      </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Australia's Qantas to pay $79m over 'ghost flights' furore | Aviation ...</t>
-        </is>
-      </c>
-      <c r="B35" s="1" t="n">
-        <v>45417</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Australia's flagship airline Qantas has agreed to pay $120 million Australian dollars ($79m) to settle a lawsuit over the sale of tickets</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>./output/33.jpg</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
-        <v>1</v>
-      </c>
-      <c r="F35" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>